<commit_message>
Uprava rozlozeni defaultniho zobrazeni, obrazky
</commit_message>
<xml_diff>
--- a/FarmaVojovice/Data/OfferList.xlsx
+++ b/FarmaVojovice/Data/OfferList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjektyGit\FarmaVojoviceWeb\FarmaVojovice\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01C6703E-D345-4A59-8412-2CA15607C7AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C094BA7-E4FB-48F5-BEE9-7423B54F961A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Jmeno</t>
   </si>
@@ -70,6 +70,18 @@
   </si>
   <si>
     <t>21.1.2022</t>
+  </si>
+  <si>
+    <t>2501 kc</t>
+  </si>
+  <si>
+    <t>21.1.2023</t>
+  </si>
+  <si>
+    <t>Balicek 5 kg</t>
+  </si>
+  <si>
+    <t>Jazyk + Jitrnice</t>
   </si>
 </sst>
 </file>
@@ -395,17 +407,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -462,6 +474,20 @@
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>